<commit_message>
CreateDb OrderDetail Add Columns
</commit_message>
<xml_diff>
--- a/CreateDb/DataDictionary.xlsx
+++ b/CreateDb/DataDictionary.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuei\Documents\Projects\DecimalFloatTailZero\CreateDb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuei\Projects\DecimalFloatTailZero\CreateDb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31561DA7-8240-4E7A-A520-849D72E09999}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95352826-4E1A-4785-9C10-C745EB14A099}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2805" yWindow="765" windowWidth="16065" windowHeight="14505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="_Template (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="_Template" sheetId="3" r:id="rId1"/>
     <sheet name="Order" sheetId="2" r:id="rId2"/>
     <sheet name="OrderDetail" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -306,7 +306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="55">
   <si>
     <t>某資料表</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -472,64 +472,78 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>小計</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>總計</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>營業稅</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nvarchar(50)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>名稱</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>備註</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>小計</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>總計</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>營業稅</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>金額</t>
+  </si>
+  <si>
+    <t>Item</t>
   </si>
   <si>
     <t>nvarchar(50)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>名稱</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>項目</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -537,7 +551,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -562,6 +576,20 @@
       <family val="3"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -586,7 +614,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
@@ -609,28 +637,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -920,7 +957,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -931,34 +968,34 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -967,7 +1004,7 @@
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -986,7 +1023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -999,17 +1036,17 @@
       <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1022,15 +1059,15 @@
       <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1041,7 +1078,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1052,63 +1089,63 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="11"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="11"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="11"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="11"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5">
       <c r="E17" s="2"/>
     </row>
   </sheetData>
@@ -1127,243 +1164,243 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED47FCF-840B-4D5F-8DBA-3CC88D4B4AA8}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="15.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="E6" s="13"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="2"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="5:5">
+      <c r="E18" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1379,249 +1416,287 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF84C242-DF0E-49D7-AF72-116061230207}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="15.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="12" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="2"/>
+      <c r="D11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="5:5">
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="5:5">
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="5:5">
+      <c r="E20" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>